<commit_message>
fixed big mistake in exercise2
</commit_message>
<xml_diff>
--- a/HW2/Exercise2.xlsx
+++ b/HW2/Exercise2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF384CA6-49E1-E941-A3EF-479A43BAE477}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DE8996-79F5-A946-B945-AEC3E8C4642B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24120" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="23460" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solution_v1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Solution_v1!$F$3:$F$16</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Solution_v1!$G$3:$G$16</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Solution_v1!$C$24:$F$24</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Year1</t>
   </si>
@@ -132,7 +132,12 @@
     <t>Interests</t>
   </si>
   <si>
-    <t>Capital</t>
+    <t>Capital
+savings</t>
+  </si>
+  <si>
+    <t>Capital
+Bonds</t>
   </si>
 </sst>
 </file>
@@ -140,10 +145,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,9 +184,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,10 +227,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="OpenSolver1">
+        <xdr:cNvPr id="3" name="OpenSolver1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D65FE82B-DE9E-3144-BEAC-C527EB49D7EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C1F2AF-C07F-6E43-9BF9-E00A30CBD30E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -220,7 +239,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2971800" y="4381500"/>
-          <a:ext cx="2654300" cy="190500"/>
+          <a:ext cx="3111500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -294,10 +313,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="OpenSolver2">
+        <xdr:cNvPr id="4" name="OpenSolver2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A621B0CF-32D4-1B4A-B3C6-0FCA953AA937}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75F84E98-9B4B-9A46-818C-A53561A21F26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -375,10 +394,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="OpenSolver3">
+        <xdr:cNvPr id="5" name="OpenSolver3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FFD05B1-47D9-2D4C-B34B-14E6468CEB0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA30AAF-BDE0-644F-A79C-8D5CC4722454}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -466,10 +485,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="OpenSolver4">
+        <xdr:cNvPr id="6" name="OpenSolver4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3342E8D-1544-B240-A306-7691C823187C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE46180C-9CAD-4740-9B3F-F292448D9D43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,23 +553,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="OpenSolver5">
+        <xdr:cNvPr id="7" name="OpenSolver5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44DD264C-2214-8A46-8F3F-DB0984D785D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E3B8EB8-2591-114D-A64D-65D31B92A991}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -558,7 +577,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953000" y="381000"/>
+          <a:off x="6083300" y="381000"/>
           <a:ext cx="673100" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -624,29 +643,29 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="OpenSolver6">
+        <xdr:cNvPr id="8" name="OpenSolver6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0897D53-3FE5-4641-B322-647F43EC75B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76DBC972-CAA7-0D44-91BC-7584199D64FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="3"/>
-          <a:endCxn id="13" idx="1"/>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="7" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3619500" y="1714500"/>
-          <a:ext cx="1333500" cy="0"/>
+          <a:ext cx="2463800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -679,23 +698,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="OpenSolver7">
+        <xdr:cNvPr id="17" name="OpenSolver7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B67CA348-0EB2-FE4E-9769-02EBB56E2789}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666C7CE0-C6DD-CD4C-A870-5B5F9AA9061D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -703,7 +722,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4095750" y="1587500"/>
+          <a:off x="4660900" y="1587500"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -777,10 +796,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="OpenSolverC24:F24">
+        <xdr:cNvPr id="18" name="OpenSolverC24:F24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12A56623-B9EF-994F-A5B0-979F0484DB8F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C032654-86D8-DB45-B2B9-06E5F7942FE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -789,7 +808,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2984500" y="4394200"/>
-          <a:ext cx="2641600" cy="177800"/>
+          <a:ext cx="3098800" cy="177800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1170,37 +1189,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G27"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="2" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="2" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1209,18 +1229,22 @@
       </c>
       <c r="D3">
         <f>SUMPRODUCT(C21:F21,C24:F24)</f>
-        <v>30.998077500000001</v>
-      </c>
-      <c r="F3">
-        <f>D3+E3</f>
-        <v>30.998077500000001</v>
+        <v>11.978074894999999</v>
+      </c>
+      <c r="E3">
+        <f>F24</f>
+        <v>9.3763039999999993</v>
       </c>
       <c r="G3">
-        <f>F3-C3</f>
-        <v>18.998077500000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+        <f>D3+E3+F3</f>
+        <v>21.354378894999996</v>
+      </c>
+      <c r="H3">
+        <f>G3-C3</f>
+        <v>9.3543788949999964</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1228,19 +1252,23 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+G3*F$21</f>
-        <v>31.758000600000003</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F16" si="0">D4+E4</f>
-        <v>31.758000600000003</v>
+        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+H3*F$21</f>
+        <v>11.977197890799999</v>
+      </c>
+      <c r="E4">
+        <f>H3</f>
+        <v>9.3543788949999964</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G16" si="1">F4-C4</f>
-        <v>17.758000600000003</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+        <f t="shared" ref="G4:G16" si="0">D4+E4+F4</f>
+        <v>21.331576785799996</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H16" si="1">G4-C4</f>
+        <v>7.3315767857999958</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1248,19 +1276,23 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+G4*F$21</f>
-        <v>31.708397524000002</v>
-      </c>
-      <c r="F5">
+        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+H4*F$21</f>
+        <v>11.896285806431999</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E16" si="2">H4</f>
+        <v>7.3315767857999958</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>31.708397524000002</v>
-      </c>
-      <c r="G5">
+        <v>19.227862592231993</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>16.708397524000002</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+        <v>4.2278625922319932</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1268,19 +1300,23 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D8" si="2">SUMPRODUCT(C$21:E$21,C$24:E$24)+G5*F$21</f>
-        <v>31.66641340096</v>
-      </c>
-      <c r="F6">
+        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+H5*F$21</f>
+        <v>11.772137238689279</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>4.2278625922319932</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>31.66641340096</v>
-      </c>
-      <c r="G6">
+        <v>15.999999830921272</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>15.66641340096</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+        <v>-1.690787279073902E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1288,23 +1324,27 @@
         <v>18</v>
       </c>
       <c r="D7">
+        <f>SUMPRODUCT(C$21:E$21,C$24:E$24)+H6*F$21</f>
+        <v>11.603022728236851</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="2"/>
-        <v>31.624734036038401</v>
-      </c>
-      <c r="E7">
+        <v>-1.690787279073902E-7</v>
+      </c>
+      <c r="F7">
         <f>C23*C24</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
+        <v>73.694798000000006</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>31.624734036038401</v>
-      </c>
-      <c r="G7">
+        <v>85.297820559158126</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>13.624734036038401</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+        <v>67.297820559158126</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1312,19 +1352,23 @@
         <v>20</v>
       </c>
       <c r="D8">
-        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+G7*F$21</f>
-        <v>31.543066861441538</v>
-      </c>
-      <c r="F8">
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H7*F$21</f>
+        <v>9.8732476773663258</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>67.297820559158126</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>31.543066861441538</v>
-      </c>
-      <c r="G8">
+        <v>77.171068236524448</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>11.543066861441538</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+        <v>57.171068236524448</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1332,19 +1376,23 @@
         <v>21</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D14" si="3">SUMPRODUCT(D$21:E$21,D$24:E$24)+G8*F$21</f>
-        <v>31.459800174457662</v>
-      </c>
-      <c r="F9">
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H8*F$21</f>
+        <v>9.4681775844609781</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>57.171068236524448</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>31.459800174457662</v>
-      </c>
-      <c r="G9">
+        <v>66.639245820985423</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>10.459800174457662</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+        <v>45.639245820985423</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1352,19 +1400,23 @@
         <v>22</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
-        <v>31.416469506978306</v>
-      </c>
-      <c r="F10">
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H9*F$21</f>
+        <v>9.0069046878394179</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>45.639245820985423</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>31.416469506978306</v>
-      </c>
-      <c r="G10">
+        <v>54.646150508824839</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>9.4164695069783058</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+        <v>32.646150508824839</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1372,19 +1424,23 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
-        <v>31.374736280279134</v>
-      </c>
-      <c r="F11">
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H10*F$21</f>
+        <v>8.487180875352994</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>32.646150508824839</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>31.374736280279134</v>
-      </c>
-      <c r="G11">
+        <v>41.133331384177836</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>7.3747362802791336</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+        <v>17.133331384177836</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1392,19 +1448,23 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
-        <v>31.293066951211166</v>
-      </c>
-      <c r="F12">
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H11*F$21</f>
+        <v>7.8666681103671134</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>17.133331384177836</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>31.293066951211166</v>
-      </c>
-      <c r="G12">
+        <v>24.999999494544952</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>6.2930669512111663</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+        <v>-5.0545504848287237E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1412,23 +1472,27 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
-        <v>31.249800178048446</v>
+        <f>SUMPRODUCT(D$21:E$21,D$24:E$24)+H12*F$21</f>
+        <v>7.181334834781798</v>
       </c>
       <c r="E13">
+        <f t="shared" si="2"/>
+        <v>-5.0545504848287237E-7</v>
+      </c>
+      <c r="F13">
         <f>D23*D24</f>
-        <v>0</v>
-      </c>
-      <c r="F13">
+        <v>77.208371999999997</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>31.249800178048446</v>
-      </c>
-      <c r="G13">
+        <v>84.389706329326742</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="1"/>
-        <v>1.2498001780484458</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+        <v>54.389706329326742</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1436,19 +1500,23 @@
         <v>31</v>
       </c>
       <c r="D14">
-        <f>E$21*E$24+G13*F$21</f>
-        <v>31.048069507121937</v>
-      </c>
-      <c r="F14">
+        <f>E$21*E$24+H13*F$21</f>
+        <v>4.3383789281730696</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>54.389706329326742</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>31.048069507121937</v>
-      </c>
-      <c r="G14">
+        <v>58.728085257499814</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="1"/>
-        <v>4.8069507121937249E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+        <v>27.728085257499814</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1456,19 +1524,23 @@
         <v>31</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D16" si="4">E$21*E$24+G14*F$21</f>
-        <v>31.00000028028488</v>
-      </c>
-      <c r="F15">
+        <f>E$21*E$24+H14*F$21</f>
+        <v>3.2719140852999926</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>27.728085257499814</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="0"/>
-        <v>31.00000028028488</v>
-      </c>
-      <c r="G15">
+        <v>30.999999342799807</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="1"/>
-        <v>2.802848797500701E-7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+        <v>-6.5720019293280529E-7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1476,20 +1548,24 @@
         <v>31</v>
       </c>
       <c r="D16">
-        <f t="shared" si="4"/>
-        <v>30.998077511211395</v>
+        <f>E$21*E$24+H15*F$21</f>
+        <v>2.1627906487119923</v>
       </c>
       <c r="E16">
+        <f t="shared" si="2"/>
+        <v>-6.5720019293280529E-7</v>
+      </c>
+      <c r="F16">
         <f>E24*E23</f>
-        <v>413.30770000000001</v>
-      </c>
-      <c r="F16">
+        <v>28.837209000000001</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="0"/>
-        <v>444.30577751121143</v>
-      </c>
-      <c r="G16">
+        <v>30.999998991511802</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
-        <v>413.30577751121143</v>
+        <v>-1.0084881978400517E-6</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -1583,17 +1659,17 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>413.30770000000001</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
+      <c r="C24" s="1">
+        <v>73.694798000000006</v>
+      </c>
+      <c r="D24" s="1">
+        <v>77.208371999999997</v>
+      </c>
+      <c r="E24" s="1">
+        <v>28.837209000000001</v>
+      </c>
+      <c r="F24" s="1">
+        <v>9.3763039999999993</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
@@ -1602,7 +1678,7 @@
       </c>
       <c r="C27" s="1">
         <f>SUMPRODUCT(C24:F24,C20:F20)</f>
-        <v>433.97308500000003</v>
+        <v>186.76839633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>